<commit_message>
finished Word document report
</commit_message>
<xml_diff>
--- a/ai_scenario_simulation/Cost_Savings_Summary.xlsx
+++ b/ai_scenario_simulation/Cost_Savings_Summary.xlsx
@@ -1,41 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucymalmud/Desktop/hazira-port/ai_scenario_simulation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3155E3-FFB6-094C-A45C-300F01FEA5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="25780" windowHeight="11000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Savings_by_subprocess" sheetId="1" r:id="rId1"/>
     <sheet name="KPI_changes" sheetId="2" r:id="rId2"/>
     <sheet name="Totals" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>subprocess</t>
   </si>
@@ -98,19 +79,13 @@
   </si>
   <si>
     <t>scenario_total_cost</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>excludes quay_crane, yard_crane, container_moves, truck_entry, energy, vessel_service_hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,21 +148,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -225,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -259,7 +226,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -294,10 +260,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -470,14 +435,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -511,25 +476,25 @@
         <v>52343.1</v>
       </c>
       <c r="C2">
-        <v>266949810</v>
+        <v>26694.981</v>
       </c>
       <c r="D2">
-        <v>48129.120000000003</v>
+        <v>48119.94</v>
       </c>
       <c r="E2">
-        <v>245458512</v>
+        <v>24541.1694</v>
       </c>
       <c r="F2">
-        <v>21491298</v>
+        <v>2153.811599999997</v>
       </c>
       <c r="G2">
-        <v>8.0506886294468616E-2</v>
+        <v>0.08068226757681518</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -537,25 +502,25 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C3">
-        <v>439975650</v>
+        <v>4399.7565</v>
       </c>
       <c r="D3">
-        <v>113967.45</v>
+        <v>114055.85</v>
       </c>
       <c r="E3">
-        <v>410282820</v>
+        <v>4106.0106</v>
       </c>
       <c r="F3">
-        <v>29692830</v>
+        <v>293.7458999999999</v>
       </c>
       <c r="G3">
-        <v>6.748743936170104E-2</v>
+        <v>0.06676412660564282</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -563,25 +528,25 @@
         <v>47753</v>
       </c>
       <c r="C4">
-        <v>18146140</v>
+        <v>181.4614</v>
       </c>
       <c r="D4">
-        <v>52532.800000000003</v>
+        <v>52475.5</v>
       </c>
       <c r="E4">
-        <v>19962464</v>
+        <v>199.4069</v>
       </c>
       <c r="F4">
-        <v>-1816324</v>
+        <v>-17.94550000000001</v>
       </c>
       <c r="G4">
-        <v>-0.100094234917178</v>
+        <v>-0.09889431030511178</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -589,25 +554,25 @@
         <v>52343.1</v>
       </c>
       <c r="C5">
-        <v>266949810</v>
+        <v>26694.981</v>
       </c>
       <c r="D5">
-        <v>47764.706666666672</v>
+        <v>47754.77166666667</v>
       </c>
       <c r="E5">
-        <v>243600004</v>
+        <v>24354.93355</v>
       </c>
       <c r="F5">
-        <v>23349806</v>
+        <v>2340.047449999998</v>
       </c>
       <c r="G5">
-        <v>8.7468899116279572E-2</v>
+        <v>0.08765870445833987</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -615,25 +580,25 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C6">
-        <v>439975650</v>
+        <v>4399.7565</v>
       </c>
       <c r="D6">
-        <v>113253.24</v>
+        <v>113348.92</v>
       </c>
       <c r="E6">
-        <v>407711664</v>
+        <v>4080.56112</v>
       </c>
       <c r="F6">
-        <v>32263986</v>
+        <v>319.1953799999997</v>
       </c>
       <c r="G6">
-        <v>7.3331299129849578E-2</v>
+        <v>0.07254841944093944</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -641,25 +606,25 @@
         <v>47753</v>
       </c>
       <c r="C7">
-        <v>18146140</v>
+        <v>181.4614</v>
       </c>
       <c r="D7">
-        <v>50622.879999999997</v>
+        <v>50567.3</v>
       </c>
       <c r="E7">
-        <v>19236694.399999999</v>
+        <v>192.15574</v>
       </c>
       <c r="F7">
-        <v>-1090554.399999999</v>
+        <v>-10.69433999999998</v>
       </c>
       <c r="G7">
-        <v>-6.0098423135719142E-2</v>
+        <v>-0.05893451720310756</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -667,25 +632,25 @@
         <v>52343.1</v>
       </c>
       <c r="C8">
-        <v>266949810</v>
+        <v>26694.981</v>
       </c>
       <c r="D8">
-        <v>47555.953333333331</v>
+        <v>47545.58583333333</v>
       </c>
       <c r="E8">
-        <v>242535362</v>
+        <v>24248.248775</v>
       </c>
       <c r="F8">
-        <v>24414448</v>
+        <v>2446.732225</v>
       </c>
       <c r="G8">
-        <v>9.1457072024138164E-2</v>
+        <v>0.09165514015537227</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -693,25 +658,25 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C9">
-        <v>439975650</v>
+        <v>4399.7565</v>
       </c>
       <c r="D9">
-        <v>112845.12</v>
+        <v>112944.96</v>
       </c>
       <c r="E9">
-        <v>406242432</v>
+        <v>4066.01856</v>
       </c>
       <c r="F9">
-        <v>33733218</v>
+        <v>333.73794</v>
       </c>
       <c r="G9">
-        <v>7.6670647568791592E-2</v>
+        <v>0.07585372963253763</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -719,19 +684,19 @@
         <v>47753</v>
       </c>
       <c r="C10">
-        <v>18146140</v>
+        <v>181.4614</v>
       </c>
       <c r="D10">
-        <v>49190.44000000001</v>
+        <v>49136.15000000001</v>
       </c>
       <c r="E10">
-        <v>18692367.199999999</v>
+        <v>186.71737</v>
       </c>
       <c r="F10">
-        <v>-546227.20000000298</v>
+        <v>-5.255970000000048</v>
       </c>
       <c r="G10">
-        <v>-3.0101564299625318E-2</v>
+        <v>-0.02896467237660487</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -743,14 +708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -767,24 +732,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
-        <v>278.73408446521159</v>
+        <v>278.7340844652116</v>
       </c>
       <c r="C2">
-        <v>22673.869166666671</v>
+        <v>20990.58638888889</v>
       </c>
       <c r="D2">
-        <v>22395.135082201461</v>
+        <v>20711.85230442368</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -792,16 +757,16 @@
         <v>52343.1</v>
       </c>
       <c r="C3">
-        <v>48129.120000000003</v>
+        <v>48119.94</v>
       </c>
       <c r="D3">
-        <v>-4213.9799999999959</v>
+        <v>-4223.159999999996</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -809,16 +774,16 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C4">
-        <v>113967.45</v>
+        <v>114055.85</v>
       </c>
       <c r="D4">
-        <v>-8248.0083333333314</v>
+        <v>-8159.608333333323</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -826,33 +791,33 @@
         <v>47753</v>
       </c>
       <c r="C5">
-        <v>52532.800000000003</v>
+        <v>52475.5</v>
       </c>
       <c r="D5">
-        <v>4779.8000000000029</v>
+        <v>4722.5</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>278.73408446521159</v>
+        <v>278.7340844652116</v>
       </c>
       <c r="C6">
-        <v>25508.10222222222</v>
+        <v>23614.4</v>
       </c>
       <c r="D6">
-        <v>25229.36813775701</v>
+        <v>23335.66591553479</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -860,16 +825,16 @@
         <v>52343.1</v>
       </c>
       <c r="C7">
-        <v>47764.706666666672</v>
+        <v>47754.77166666667</v>
       </c>
       <c r="D7">
-        <v>-4578.3933333333334</v>
+        <v>-4588.328333333331</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -877,16 +842,16 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C8">
-        <v>113253.24</v>
+        <v>113348.92</v>
       </c>
       <c r="D8">
-        <v>-8962.2183333333232</v>
+        <v>-8866.53833333333</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -894,33 +859,33 @@
         <v>47753</v>
       </c>
       <c r="C9">
-        <v>50622.879999999997</v>
+        <v>50567.3</v>
       </c>
       <c r="D9">
-        <v>2869.8799999999969</v>
+        <v>2814.299999999996</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10">
-        <v>278.73408446521159</v>
+        <v>278.7340844652116</v>
       </c>
       <c r="C10">
-        <v>26925.22</v>
+        <v>24926.31166666667</v>
       </c>
       <c r="D10">
-        <v>26646.485915534791</v>
+        <v>24647.57758220146</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -928,16 +893,16 @@
         <v>52343.1</v>
       </c>
       <c r="C11">
-        <v>47555.953333333331</v>
+        <v>47545.58583333333</v>
       </c>
       <c r="D11">
-        <v>-4787.1466666666674</v>
+        <v>-4797.514166666668</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -945,16 +910,16 @@
         <v>122215.4583333333</v>
       </c>
       <c r="C12">
-        <v>112845.12</v>
+        <v>112944.96</v>
       </c>
       <c r="D12">
-        <v>-9370.3383333333331</v>
+        <v>-9270.498333333337</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -962,10 +927,10 @@
         <v>47753</v>
       </c>
       <c r="C13">
-        <v>49190.44000000001</v>
+        <v>49136.15000000001</v>
       </c>
       <c r="D13">
-        <v>1437.4400000000101</v>
+        <v>1383.150000000009</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -977,24 +942,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1008,69 +963,57 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>725071600</v>
+        <v>31276.1989</v>
       </c>
       <c r="B2">
-        <v>675703796</v>
+        <v>28846.5869</v>
       </c>
       <c r="C2">
-        <v>49367804</v>
+        <v>2429.611999999997</v>
       </c>
       <c r="D2">
-        <v>6.8086798600303755E-2</v>
+        <v>0.07768245776183491</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
-        <v>725071600</v>
+        <v>31276.1989</v>
       </c>
       <c r="B3">
-        <v>670548362.39999998</v>
+        <v>28627.65041</v>
       </c>
       <c r="C3">
-        <v>54523237.600000001</v>
+        <v>2648.548489999998</v>
       </c>
       <c r="D3">
-        <v>7.5197039299291266E-2</v>
+        <v>0.08468255680520045</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
-        <v>725071600</v>
+        <v>31276.1989</v>
       </c>
       <c r="B4">
-        <v>667470161.20000005</v>
+        <v>28500.984705</v>
       </c>
       <c r="C4">
-        <v>57601438.799999997</v>
+        <v>2775.214195</v>
       </c>
       <c r="D4">
-        <v>7.9442414790484139E-2</v>
+        <v>0.08873246406551021</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>